<commit_message>
one to one mapping
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ram\classes\workspace\Hibernate\Sep_18_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A74DCDDB-8AD1-42EF-AFF8-0EF83AB9C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EB6242-F92A-41F8-B502-43EBC3436CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{48355570-7748-4DC4-82AF-538498E23569}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="21480" windowHeight="15585" activeTab="3" xr2:uid="{48355570-7748-4DC4-82AF-538498E23569}"/>
   </bookViews>
   <sheets>
     <sheet name="01_demo" sheetId="1" r:id="rId1"/>
     <sheet name="05_embedded" sheetId="2" r:id="rId2"/>
     <sheet name="07_collection" sheetId="3" r:id="rId3"/>
+    <sheet name="mapping" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
   <si>
     <t>Employee</t>
   </si>
@@ -145,6 +146,140 @@
   </si>
   <si>
     <t>emp_projects</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>last_updated</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>One to One</t>
+  </si>
+  <si>
+    <t>One to Many /Many to One</t>
+  </si>
+  <si>
+    <t>Many to Many</t>
+  </si>
+  <si>
+    <t>@Entity
+class Employee{
+  String id;
+  Address address;
+}</t>
+  </si>
+  <si>
+    <t>@Entity
+class Address{
+ Long addressId;
+ String city;
+ String pincode;
+}</t>
+  </si>
+  <si>
+    <t>addressId</t>
+  </si>
+  <si>
+    <t>pinCode</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Many emp can work in one dept</t>
+  </si>
+  <si>
+    <t>@Entity
+class Employee{
+  String id;
+  Department dept;
+}</t>
+  </si>
+  <si>
+    <t>@Entity
+class Department{
+ Long deptId;
+ String departmentName;
+}</t>
+  </si>
+  <si>
+    <t>add_id</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>dname</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>@Entity
+class Employee{
+  String id;
+  List&lt;Project&gt;  projects;
+}</t>
+  </si>
+  <si>
+    <t>@Entity
+class Project{
+ Long projectId;
+ String projectName;
+ String client;
+}</t>
+  </si>
+  <si>
+    <t>projectId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>Infosys</t>
+  </si>
+  <si>
+    <t>TMS</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Passport</t>
   </si>
 </sst>
 </file>
@@ -160,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +305,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,15 +357,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -226,7 +367,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,38 +689,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4C38C5-2700-41B3-A876-04E953A5CFEB}">
-  <dimension ref="B1:F6"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -585,8 +735,14 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -594,7 +750,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -602,13 +758,57 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -625,7 +825,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+      <selection activeCell="I4" sqref="I4:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,26 +844,26 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -728,24 +928,24 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
@@ -792,18 +992,18 @@
       <c r="I14" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
@@ -906,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079645E7-3B9F-4F58-8ED6-BA7E3B0822CA}">
   <dimension ref="B2:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3:M6"/>
     </sheetView>
   </sheetViews>
@@ -917,14 +1117,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -939,7 +1139,6 @@
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7"/>
       <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1050,4 +1249,485 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E33ECF9-A23C-4D6F-AFE7-F446A2DFB124}">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1001</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1">
+        <v>411041</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1002</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1">
+        <v>41111</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1001</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1001</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="1">
+        <v>411041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1002</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1002</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="1">
+        <v>41111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1001</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="1">
+        <v>411041</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1002</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1002</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="1">
+        <v>41111</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>20</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1001</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1002</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B16:C16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>